<commit_message>
Testes de junho 2022
</commit_message>
<xml_diff>
--- a/mapeamentos-ind.xlsx
+++ b/mapeamentos-ind.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\OneDrive\Prefeitura\2022\MSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\OneDrive\Prefeitura\2022\MSC\conferencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C841DCE-C6A9-4DB6-9646-B5DF15C2842B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA79B5F-6B15-47E8-9251-4BE70A1849AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{290FD983-6FC8-434A-8650-042E2310D2E9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3068" uniqueCount="1692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3072" uniqueCount="1694">
   <si>
     <t>Código TCE</t>
   </si>
@@ -5111,6 +5111,12 @@
   </si>
   <si>
     <t>2.1.1.4.2.02.01.01.02.00</t>
+  </si>
+  <si>
+    <t>1.1.9.8.1.01.02.</t>
+  </si>
+  <si>
+    <t>1.1.9.8.1.01.04.</t>
   </si>
 </sst>
 </file>
@@ -5172,8 +5178,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5012BCD-765A-4258-ACCE-F25621784DF0}" name="Tabela1" displayName="Tabela1" ref="A1:B1534" totalsRowShown="0">
-  <autoFilter ref="A1:B1534" xr:uid="{C5012BCD-765A-4258-ACCE-F25621784DF0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5012BCD-765A-4258-ACCE-F25621784DF0}" name="Tabela1" displayName="Tabela1" ref="A1:B1536" totalsRowShown="0">
+  <autoFilter ref="A1:B1536" xr:uid="{C5012BCD-765A-4258-ACCE-F25621784DF0}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{727D9B8B-C562-4F54-89D8-0C965F1407B0}" name="Código TCE"/>
     <tableColumn id="2" xr3:uid="{4826B92B-3D33-462D-BAC9-C9E7438F2575}" name="Código STN"/>
@@ -5479,10 +5485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0915C7-1FF0-4F18-90C3-17A9D9021303}">
-  <dimension ref="A1:B1534"/>
+  <dimension ref="A1:B1536"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1510" workbookViewId="0">
-      <selection activeCell="A1529" sqref="A1529"/>
+      <selection activeCell="A1537" sqref="A1537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17763,6 +17769,22 @@
         <v>1684</v>
       </c>
     </row>
+    <row r="1535" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1535" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B1535" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1536" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B1536" t="s">
+        <v>1558</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>